<commit_message>
updated DPP master file export to include 2nd table
</commit_message>
<xml_diff>
--- a/masterTemplate.xlsx
+++ b/masterTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\redcap\plugins\dprp-cdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11C7212-C30E-4ADF-8F1E-08E11A0C913A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996B6E87-8618-47A9-82E2-6DC25AA893C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-3770" windowWidth="38620" windowHeight="21220" xr2:uid="{B89E40F1-3C2E-4611-9151-93A28888AD76}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B89E40F1-3C2E-4611-9151-93A28888AD76}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="1" r:id="rId1"/>
@@ -113,10 +113,6 @@
     <t>SESSION 16 09/24/2019</t>
   </si>
   <si>
-    <t>SESSION 17
-10/01/2019</t>
-  </si>
-  <si>
     <t>SESSION 18 10/17/2019</t>
   </si>
   <si>
@@ -151,6 +147,9 @@
   </si>
   <si>
     <t>SESSION 1 04/23/2019</t>
+  </si>
+  <si>
+    <t>SESSION 17 10/01/2019</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1096,7 @@
   <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P49" sqref="P48:P49"/>
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,7 +1135,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1193,40 +1192,40 @@
         <v>20</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="AJ1" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
replaced hard-coded column references with initialized values
</commit_message>
<xml_diff>
--- a/masterTemplate.xlsx
+++ b/masterTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\redcap\plugins\dprp-cdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996B6E87-8618-47A9-82E2-6DC25AA893C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701CF512-3E7D-42D3-8798-084C00AFB86F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B89E40F1-3C2E-4611-9151-93A28888AD76}"/>
+    <workbookView xWindow="5505" yWindow="2175" windowWidth="21600" windowHeight="11385" xr2:uid="{B89E40F1-3C2E-4611-9151-93A28888AD76}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1096,7 +1097,7 @@
   <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added instructions and legend sheets to workbook template file
</commit_message>
<xml_diff>
--- a/masterTemplate.xlsx
+++ b/masterTemplate.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\redcap\plugins\dprp-cdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701CF512-3E7D-42D3-8798-084C00AFB86F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A488ACE-DA95-4073-A8E2-C3FB98022E64}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5505" yWindow="2175" windowWidth="21600" windowHeight="11385" xr2:uid="{B89E40F1-3C2E-4611-9151-93A28888AD76}"/>
+    <workbookView xWindow="19090" yWindow="-3770" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{B89E40F1-3C2E-4611-9151-93A28888AD76}"/>
   </bookViews>
   <sheets>
-    <sheet name="Combined" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="2" r:id="rId1"/>
+    <sheet name="Legend" sheetId="3" r:id="rId2"/>
+    <sheet name="Header" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_Hlk18856098" localSheetId="0">Instructions!$A$12</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>LAST NAME</t>
   </si>
@@ -39,9 +44,6 @@
     <t>FIRST NAME</t>
   </si>
   <si>
-    <t>EMPLOYEE ID</t>
-  </si>
-  <si>
     <t>ORG</t>
   </si>
   <si>
@@ -151,6 +153,790 @@
   </si>
   <si>
     <t>SESSION 17 10/01/2019</t>
+  </si>
+  <si>
+    <t>Instructions for DPP Coach Workbooks</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fill in all scheduled dates for DPP sessions in the first row of each table.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dates should be entered in the same cell as the session number (the row that is in bold).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Table 1: Weight</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, enter the weight for each participant at each session.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If a participant misses a session and you do not have a weight measurement for that session, leave the cell blank.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If a participant attends a session but they choose not to record a weight for that session, leave the cell blank.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Table 2: Physical Activity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, enter the physical activity minutes reported for each participant at each session.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If a participant misses a session and you do not have physical activity minutes reported for that session, leave the cell blank.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If a participant attends a session but they choose not to report physical activity minutes for that session, do not enter any numbers in the corresponding cell. Just enter the letter “A” in the corresponding cell.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Make-up Sessions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: If a participant misses a scheduled DPP session but completes a make-up session, follow these instructions:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Table 1: Weight</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, record the participant’s weight for the corresponding session.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                               </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If a participant chooses not to record a weight for the make-up session, leave the cell blank.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Table 2: Physical Activity</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                               </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Enter the physical activity minutes reported by the participant for that session in the corresponding cell followed by a comma.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If a participant chooses not to record physical activity minutes for the make-up session, do not enter any numbers in the corresponding cell. Just enter the letter “A” in the corresponding cell.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ii.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>After the comma, type the date that the participant completed the make-up session followed by another comma</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                           </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>iii.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>After the comma, type one of the following letters to indicate how the participant completed the make-up session</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I: In-person (met with coach in-person to complete make-up session)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>O: Online (independently completed make-up module in REDCap)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D: Distance Learning (met with coach via phone or Zoom to complete make-up session)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                           </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>iv.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Highlight the cell in yellow</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For example, if a participant missed session 8 which was scheduled for September 3, 2019 but did a make-up session by herself using the REDCap module on September 5, 2019 (weight 180 lbs, physical activity 120 minutes), you would document the following</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                               </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>In Table 1, record “180” in the cell for session 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ii.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>In Table 2, record “120, 09/05/2019, O” in the cell for session 8 and highlight the cell yellow</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Miscellaneous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Do not delete any participant from the excel spreadsheet or move their row of data to a different location on the spreadsheet. If they drop out or stop attending, just leave the cells blank for any sessions they do not attend.</t>
+    </r>
+  </si>
+  <si>
+    <t>Enter physical activity minutes then comma</t>
+  </si>
+  <si>
+    <t>Enter date of make-up session then comma</t>
+  </si>
+  <si>
+    <t>Enter I, O, or D for type of make-up session</t>
+  </si>
+  <si>
+    <t>Highlight the cell in yellow</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>If did not attend a session, leave the weight and physical activity minute cells blank</t>
+  </si>
+  <si>
+    <t>If attended but missing weight data, leave the cell blank in Table 1</t>
+  </si>
+  <si>
+    <t>If attended but missing physical activity data, enter the letter “A” (instead of numbers) in Table 2</t>
+  </si>
+  <si>
+    <t>If completed a make-up session instead of scheduled session do the following in Table 2:</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
   </si>
 </sst>
 </file>
@@ -160,7 +946,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +1095,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -697,7 +1498,7 @@
     <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -714,14 +1515,36 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="10"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="58">
@@ -1093,50 +1916,265 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533A408D-1F85-4A52-ACD7-D2870C8DB10B}">
-  <dimension ref="A1:AN1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BA50E9-45ED-4377-8878-2080F5B2E268}">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:K36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A561AEE-E257-4291-8FA7-E55B0382A878}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="D53" sqref="D53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533A408D-1F85-4A52-ACD7-D2870C8DB10B}">
+  <dimension ref="A1:AM1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="35" width="11" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="34" width="11" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1178,22 +2216,22 @@
         <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>27</v>
@@ -1226,7 +2264,7 @@
         <v>36</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="AJ1" s="1" t="s">
         <v>21</v>
@@ -1237,11 +2275,8 @@
       <c r="AL1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="AN1" s="7" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added coach_cohort page, added coach and cohort dropdowns, updated masterTemplate
</commit_message>
<xml_diff>
--- a/masterTemplate.xlsx
+++ b/masterTemplate.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\redcap\plugins\dprp-cdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A488ACE-DA95-4073-A8E2-C3FB98022E64}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92F2225-9559-40D5-A4F0-6DB7B90186A5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-3770" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{B89E40F1-3C2E-4611-9151-93A28888AD76}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
-    <sheet name="Legend" sheetId="3" r:id="rId2"/>
-    <sheet name="Header" sheetId="1" r:id="rId3"/>
+    <sheet name="Header" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_Hlk18856098" localSheetId="0">Instructions!$A$12</definedName>
@@ -1917,10 +1916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BA50E9-45ED-4377-8878-2080F5B2E268}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:K36"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2005,52 +2004,109 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="14"/>
     </row>
   </sheetData>
@@ -2060,82 +2116,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A561AEE-E257-4291-8FA7-E55B0382A878}">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533A408D-1F85-4A52-ACD7-D2870C8DB10B}">
   <dimension ref="A1:AM1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added participant ID to workbook
</commit_message>
<xml_diff>
--- a/masterTemplate.xlsx
+++ b/masterTemplate.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\redcap\plugins\dprp-cdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8C65B31-88B7-46F2-8F13-10194F9A29AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEB96CA-894A-4EC0-84BD-2E7801124335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-3770" windowWidth="38620" windowHeight="21220" firstSheet="1" activeTab="1" xr2:uid="{B89E40F1-3C2E-4611-9151-93A28888AD76}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B89E40F1-3C2E-4611-9151-93A28888AD76}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
     <sheet name="Header" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_Hlk18856098" localSheetId="0">Instructions!$A$12</definedName>
+    <definedName name="_Hlk18856098" localSheetId="0">Instructions!$A$13</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Instructions for DPP Coach Workbooks</t>
   </si>
@@ -937,6 +937,67 @@
   </si>
   <si>
     <t>Total sessions attended</t>
+  </si>
+  <si>
+    <t>PARTICIPANT ID</t>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Format days as mm/dd/yyyy (e.g., January 3rd, 2020 would be 01/03/2020).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>iii.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If you happen to enter only a date in a second table cell, prevent Excel from turning the cell into a Date format by adding an apostrophe before the date value. (e.g., 5/2/2019 =&gt; '5/2/2019)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -946,7 +1007,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1917,198 +1978,208 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BA50E9-45ED-4377-8878-2080F5B2E268}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="11" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="11" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="10" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="11" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="11" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="12" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="11" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="12" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="13" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="12" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="12" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="13" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="13" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="13" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="12" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="11" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="12" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="12" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="10" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="9" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="16" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="16" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="16" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="16" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="C32" s="8" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
-      <c r="C33" s="8" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
-      <c r="C34" s="8" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
-      <c r="C35" s="15" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
-      <c r="B37" s="14"/>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2118,150 +2189,154 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533A408D-1F85-4A52-ACD7-D2870C8DB10B}">
-  <dimension ref="A1:AM1"/>
+  <dimension ref="A1:AN1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="34" width="11" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="35" width="11" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="45">
+    <row r="1" spans="1:40" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AN1" s="6" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>